<commit_message>
inheritance and access priviilege
</commit_message>
<xml_diff>
--- a/java_latest_st.xlsx
+++ b/java_latest_st.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5680" uniqueCount="3081">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5699" uniqueCount="3092">
   <si>
     <t>USER</t>
   </si>
@@ -9548,6 +9548,39 @@
   </si>
   <si>
     <t>====</t>
+  </si>
+  <si>
+    <t>com</t>
+  </si>
+  <si>
+    <t>shopping</t>
+  </si>
+  <si>
+    <t>cart</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>changepasswor</t>
+  </si>
+  <si>
+    <t>auth</t>
+  </si>
+  <si>
+    <t>com.amazon.shopping.*</t>
   </si>
 </sst>
 </file>
@@ -21243,8 +21276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:V272"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21588,8 +21621,8 @@
         <v>741</v>
       </c>
     </row>
-    <row r="66" spans="9:21" ht="15.75" thickBot="1"/>
-    <row r="67" spans="9:21">
+    <row r="66" spans="2:21" ht="15.75" thickBot="1"/>
+    <row r="67" spans="2:21">
       <c r="I67" s="30"/>
       <c r="J67" s="31"/>
       <c r="K67" s="31"/>
@@ -21604,7 +21637,7 @@
       <c r="T67" s="31"/>
       <c r="U67" s="32"/>
     </row>
-    <row r="68" spans="9:21" ht="15.75" thickBot="1">
+    <row r="68" spans="2:21" ht="15.75" thickBot="1">
       <c r="I68" s="33"/>
       <c r="J68" s="27"/>
       <c r="K68" s="27"/>
@@ -21619,7 +21652,7 @@
       <c r="T68" s="27"/>
       <c r="U68" s="34"/>
     </row>
-    <row r="69" spans="9:21">
+    <row r="69" spans="2:21">
       <c r="I69" s="33"/>
       <c r="J69" s="27" t="s">
         <v>551</v>
@@ -21640,7 +21673,7 @@
       <c r="T69" s="27"/>
       <c r="U69" s="34"/>
     </row>
-    <row r="70" spans="9:21">
+    <row r="70" spans="2:21">
       <c r="I70" s="33"/>
       <c r="J70" s="27"/>
       <c r="K70" s="27"/>
@@ -21659,7 +21692,7 @@
       <c r="T70" s="27"/>
       <c r="U70" s="34"/>
     </row>
-    <row r="71" spans="9:21">
+    <row r="71" spans="2:21">
       <c r="I71" s="33"/>
       <c r="J71" s="27"/>
       <c r="K71" s="27"/>
@@ -21678,7 +21711,7 @@
       <c r="T71" s="27"/>
       <c r="U71" s="34"/>
     </row>
-    <row r="72" spans="9:21">
+    <row r="72" spans="2:21">
       <c r="I72" s="33"/>
       <c r="J72" s="27"/>
       <c r="K72" s="27"/>
@@ -21697,7 +21730,7 @@
       <c r="T72" s="51"/>
       <c r="U72" s="75"/>
     </row>
-    <row r="73" spans="9:21" ht="15.75" thickBot="1">
+    <row r="73" spans="2:21" ht="15.75" thickBot="1">
       <c r="I73" s="33"/>
       <c r="J73" s="27"/>
       <c r="K73" s="27"/>
@@ -21716,7 +21749,7 @@
       <c r="T73" s="51"/>
       <c r="U73" s="34"/>
     </row>
-    <row r="74" spans="9:21">
+    <row r="74" spans="2:21">
       <c r="I74" s="33"/>
       <c r="J74" s="27"/>
       <c r="K74" s="27"/>
@@ -21731,7 +21764,7 @@
       <c r="T74" s="51"/>
       <c r="U74" s="34"/>
     </row>
-    <row r="75" spans="9:21" ht="15.75" thickBot="1">
+    <row r="75" spans="2:21" ht="15.75" thickBot="1">
       <c r="I75" s="35"/>
       <c r="J75" s="36"/>
       <c r="K75" s="36"/>
@@ -21746,7 +21779,7 @@
       <c r="T75" s="36"/>
       <c r="U75" s="37"/>
     </row>
-    <row r="77" spans="9:21">
+    <row r="77" spans="2:21">
       <c r="I77" t="s">
         <v>745</v>
       </c>
@@ -21757,7 +21790,22 @@
         <v>748</v>
       </c>
     </row>
-    <row r="78" spans="9:21">
+    <row r="78" spans="2:21">
+      <c r="B78" t="s">
+        <v>3081</v>
+      </c>
+      <c r="C78" t="s">
+        <v>2909</v>
+      </c>
+      <c r="D78" t="s">
+        <v>3082</v>
+      </c>
+      <c r="E78" t="s">
+        <v>3083</v>
+      </c>
+      <c r="F78" t="s">
+        <v>225</v>
+      </c>
       <c r="J78" t="s">
         <v>746</v>
       </c>
@@ -21768,7 +21816,10 @@
         <v>749</v>
       </c>
     </row>
-    <row r="79" spans="9:21">
+    <row r="79" spans="2:21">
+      <c r="F79" t="s">
+        <v>3084</v>
+      </c>
       <c r="I79" t="s">
         <v>146</v>
       </c>
@@ -21776,42 +21827,89 @@
         <v>710</v>
       </c>
     </row>
-    <row r="80" spans="9:21">
+    <row r="80" spans="2:21">
+      <c r="B80" t="s">
+        <v>3081</v>
+      </c>
+      <c r="C80" t="s">
+        <v>2909</v>
+      </c>
+      <c r="D80" t="s">
+        <v>3082</v>
+      </c>
+      <c r="E80" t="s">
+        <v>3082</v>
+      </c>
       <c r="N80" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="82" spans="10:10">
+    <row r="81" spans="2:10">
+      <c r="F81" t="s">
+        <v>3085</v>
+      </c>
+    </row>
+    <row r="82" spans="2:10">
+      <c r="F82" t="s">
+        <v>3086</v>
+      </c>
       <c r="J82" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="87" spans="10:10">
+    <row r="83" spans="2:10">
+      <c r="B83" t="s">
+        <v>3081</v>
+      </c>
+      <c r="C83" t="s">
+        <v>2909</v>
+      </c>
+      <c r="D83" t="s">
+        <v>3090</v>
+      </c>
+      <c r="E83" t="s">
+        <v>3087</v>
+      </c>
+    </row>
+    <row r="84" spans="2:10">
+      <c r="F84" t="s">
+        <v>3088</v>
+      </c>
+    </row>
+    <row r="85" spans="2:10">
+      <c r="F85" t="s">
+        <v>3089</v>
+      </c>
+    </row>
+    <row r="87" spans="2:10">
+      <c r="B87" t="s">
+        <v>3091</v>
+      </c>
       <c r="J87" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="88" spans="10:10">
+    <row r="88" spans="2:10">
       <c r="J88" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="89" spans="10:10">
+    <row r="89" spans="2:10">
       <c r="J89" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="93" spans="10:10">
+    <row r="93" spans="2:10">
       <c r="J93" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="94" spans="10:10">
+    <row r="94" spans="2:10">
       <c r="J94" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="95" spans="10:10">
+    <row r="95" spans="2:10">
       <c r="J95" t="s">
         <v>794</v>
       </c>
@@ -50817,8 +50915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D3:H121"/>
   <sheetViews>
-    <sheetView topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>